<commit_message>
added config file + read from config func + tests
</commit_message>
<xml_diff>
--- a/Documents/test_requirement_map.xlsx
+++ b/Documents/test_requirement_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiha\OneDrive - post.bgu.ac.il\שולחן העבודה\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayan\Desktop\version 3\MarketSystemRepo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A249C23-9018-42E0-90A6-0BAE8CB657AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6071CFAD-12C5-4056-A204-E0F66490C1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5AAA1A21-C7B5-4175-94AF-BD01E7E4DD12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5AAA1A21-C7B5-4175-94AF-BD01E7E4DD12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="216">
   <si>
     <t>Test</t>
   </si>
@@ -50,66 +50,6 @@
     <t>store_user_tests</t>
   </si>
   <si>
-    <t>add_product_to_basket_success Passed</t>
-  </si>
-  <si>
-    <t>Check_Delivery_Success Passed</t>
-  </si>
-  <si>
-    <t>Check_Out_Failure Passed</t>
-  </si>
-  <si>
-    <t>Check_Out_Success Passed</t>
-  </si>
-  <si>
-    <t>Login_guest_test_success Passed</t>
-  </si>
-  <si>
-    <t>Login_user_test_failure Passed</t>
-  </si>
-  <si>
-    <t>Login_user_test_success Passed</t>
-  </si>
-  <si>
-    <t>Logout_user_test_failure_1 Passed</t>
-  </si>
-  <si>
-    <t>Logout_user_test_failure_2 Passed</t>
-  </si>
-  <si>
-    <t>Logout_user_test_failure_3 Passed</t>
-  </si>
-  <si>
-    <t>Logout_user_test_success Passed</t>
-  </si>
-  <si>
-    <t>register_user_test_failure Passed</t>
-  </si>
-  <si>
-    <t>register_user_test_success Passed</t>
-  </si>
-  <si>
-    <t>remove_product_from_basket_and_nothing_remains_in_it Passed</t>
-  </si>
-  <si>
-    <t>remove_product_from_basket_and_remains_some_products Passed</t>
-  </si>
-  <si>
-    <t>remove_product_from_not_existing_basket Passed</t>
-  </si>
-  <si>
-    <t>user_changes_password_fail Passed</t>
-  </si>
-  <si>
-    <t>user_changes_password_success Passed</t>
-  </si>
-  <si>
-    <t>user_purchase_history_fail Passed</t>
-  </si>
-  <si>
-    <t>user_purchase_history_success Passed</t>
-  </si>
-  <si>
     <t>StoreUnitTest</t>
   </si>
   <si>
@@ -128,189 +68,6 @@
     <t>StoreFacadeUnitTests</t>
   </si>
   <si>
-    <t>AddNewStoreStoreFacadeTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>CalculatePriceStoreFacadeTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>GatherStoresWithProductsByItemsStoreFacadeTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>PurchaseCannotPurchaseStoreFacadeTestFail Passed</t>
-  </si>
-  <si>
-    <t>PurchaseStoreFacadeTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>RemoveStoreNotFounderStoreFacadeTestFail Passed</t>
-  </si>
-  <si>
-    <t>RemoveStoreStoreFacadeTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>RestoreStoreNotFounderStoreFacadeTestFail Passed</t>
-  </si>
-  <si>
-    <t>RestoreStoreStoreFacadeTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>AddEmployeePermissionNoPermissionStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AddEmployeePermissionStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>AddProductNoPermissionStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AddProductStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>AddStorePurchasePolicyAlreadyExistsStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AddStorePurchasePolicyNoPermissionStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AddStorePurchasePolicyStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>AddStorePurchaseStrategyNoPermissionStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AddStorePurchaseStrategyStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AddStorePurchaseStrategyStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>AssignNewManagerAlreadyManagerStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AssignNewManagerStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>AssignNewManagerWithNotOwnerStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AssignNewOwnerAlreadyOwnerStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>AssignNewOwnerStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>AssignNewOwnerWithNoOwnerStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>CalculatePriceNoSuchProductStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>CalculatePriceStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>ChangeNameByFounderStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>ChangeNameByNOTFounderStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>GetItemsNoProductsInStoreStoreTest Passed</t>
-  </si>
-  <si>
-    <t>GetItemsStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>GetManagersOfTheStoreNoPermissionTestFail Passed</t>
-  </si>
-  <si>
-    <t>GetManagersOfTheStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>GetOwnersOfTheStoreNoPermissionTestFail Passed</t>
-  </si>
-  <si>
-    <t>GetOwnersOfTheStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>GetPurchaseHistoryOfTheStoreNoPermissionTestFail Passed</t>
-  </si>
-  <si>
-    <t>GetPurchaseHistoryOfTheStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>GetStoreDTOStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>ManagePermissionsStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>ManagePermissionsWithBadAssigneeStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>ManagePermissionsWithNotOwnerStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>PurchaseNorEnoughInStockStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>PurchaseStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>RemoveEmployeePermissionNoPermissionStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>RemoveEmployeePermissionStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>RemoveProductNoPermissionStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>RemoveProductNoSuchProductStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>RemoveProductStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>RemoveStoreNoFounderTest Passed</t>
-  </si>
-  <si>
-    <t>RemoveStorePurchasePolicyDoesntExistStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>RemoveStorePurchasePolicySNopermissiontoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>RemoveStorePurchasePolicyStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>RemoveStorePurchaseStrategyDoesntExistStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>RemoveStorePurchaseStrategyNoPermissionStoreTestFail Passed</t>
-  </si>
-  <si>
-    <t>RemoveStorePurchaseStrategyStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>RemoveStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>TransferFoundershipWithFounderStoreTestSuccess Passed</t>
-  </si>
-  <si>
-    <t>TransferFoundershipWithNotFounderStoreTesFailt Passed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class: store_user_tests Passed </t>
-  </si>
-  <si>
-    <t>Class: StoreFacadeUnitTests Passed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class: StoreUnitTest Passed </t>
-  </si>
-  <si>
     <t>classes beeing tested</t>
   </si>
   <si>
@@ -323,9 +80,6 @@
     <t>all</t>
   </si>
   <si>
-    <t>todo</t>
-  </si>
-  <si>
     <t>ACCEPTANCE TESTS</t>
   </si>
   <si>
@@ -906,6 +660,30 @@
   </si>
   <si>
     <t xml:space="preserve">AssignNewManagerAlreadyManagerStoreTestFail </t>
+  </si>
+  <si>
+    <t>INIT_config_tests</t>
+  </si>
+  <si>
+    <t>read_from_init_success</t>
+  </si>
+  <si>
+    <t>read_from_init_fail</t>
+  </si>
+  <si>
+    <t>read_from_config_success</t>
+  </si>
+  <si>
+    <t>2.a.i</t>
+  </si>
+  <si>
+    <t>2.a.ii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serviceLayer, market_system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">serviceLayer, PaymentProxy , DeliveryProxy </t>
   </si>
 </sst>
 </file>
@@ -916,7 +694,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -924,7 +702,7 @@
       <u/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -933,14 +711,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -965,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -979,7 +757,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,7 +775,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1296,20 +1073,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547AF65F-50E2-4545-8A86-E31EA8FDF2EA}">
   <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E204" sqref="E204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.33203125" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" customWidth="1"/>
+    <col min="1" max="1" width="75.296875" customWidth="1"/>
+    <col min="2" max="2" width="35.296875" customWidth="1"/>
+    <col min="3" max="3" width="32.19921875" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="48.109375" customWidth="1"/>
+    <col min="5" max="5" width="48.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1317,974 +1094,974 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>1.3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3">
         <v>1.3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
         <v>4.5999999999999996</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3">
         <v>4.1100000000000003</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3">
         <v>4.1100000000000003</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3">
         <v>4.1100000000000003</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C12" s="3">
         <v>4.1100000000000003</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3">
         <v>3.3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C14" s="3">
         <v>1.4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3">
         <v>1.4</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3">
         <v>1.4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3">
         <v>1.3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C18" s="3">
         <v>1.4</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C19" s="3">
         <v>1.4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3">
         <v>1.2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C21" s="3">
         <v>3.2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C22" s="3">
         <v>1.2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C23" s="3">
         <v>1.3</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C24" s="3">
         <v>4.5</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C25" s="3">
         <v>4.5</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C26" s="3">
         <v>6.2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3">
         <v>6.2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C28" s="3">
         <v>6.6</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C29" s="3">
         <v>6.6</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A30" s="6"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A33" s="6"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C34" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C36" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C37" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C38" s="3">
         <v>3.2</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C40" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C41" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C42" s="3">
         <v>3.2</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A43" s="6"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>134</v>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>140</v>
+        <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>136</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="C46" s="3">
         <v>1.3</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
-        <v>137</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="C47" s="3">
         <v>1.4</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
-        <v>138</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="C48" s="3">
         <v>1.4</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
-        <v>139</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="C49" s="3">
         <v>1.2</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>141</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="C50" s="3">
         <v>1.2</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A51" s="6"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>143</v>
+        <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C53" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E53" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C54" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E54" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C55" s="3">
         <v>2.5</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E55" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C56" s="3">
         <v>4.13</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E56" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C57" s="3">
         <v>3.7</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>66</v>
       </c>
       <c r="B58" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C59" s="3">
         <v>2.2000000000000002</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E59" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C60" s="3">
         <v>2.2000000000000002</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E60" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C61" s="3">
         <v>2.2000000000000002</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E61" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C62" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E62" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A63" s="6"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>156</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
         <v>2</v>
@@ -2293,15 +2070,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E65" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="B66" t="s">
         <v>2</v>
@@ -2310,32 +2087,32 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E66" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>76</v>
       </c>
       <c r="B67" t="s">
         <v>2</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>206</v>
+        <v>124</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E67" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
         <v>2</v>
@@ -2344,32 +2121,32 @@
         <v>3.3</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E68" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
         <v>2</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>206</v>
+        <v>124</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E69" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="B70" t="s">
         <v>2</v>
@@ -2378,15 +2155,15 @@
         <v>4.2</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E70" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>162</v>
+        <v>80</v>
       </c>
       <c r="B71" t="s">
         <v>2</v>
@@ -2395,15 +2172,15 @@
         <v>4.2</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E71" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
         <v>2</v>
@@ -2412,15 +2189,15 @@
         <v>4.3</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>82</v>
       </c>
       <c r="B73" t="s">
         <v>2</v>
@@ -2429,15 +2206,15 @@
         <v>4.3</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E73" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="B74" t="s">
         <v>2</v>
@@ -2446,49 +2223,49 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E74" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
       <c r="B75" t="s">
         <v>2</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>207</v>
+        <v>125</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E75" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>167</v>
+        <v>85</v>
       </c>
       <c r="B76" t="s">
         <v>2</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>207</v>
+        <v>125</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E76" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>168</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
         <v>2</v>
@@ -2497,15 +2274,15 @@
         <v>2.5</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E77" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>169</v>
+        <v>87</v>
       </c>
       <c r="B78" t="s">
         <v>2</v>
@@ -2514,15 +2291,15 @@
         <v>2.5</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E78" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>170</v>
+        <v>88</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
@@ -2531,15 +2308,15 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E79" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>171</v>
+        <v>89</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -2548,15 +2325,15 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E80" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>172</v>
+        <v>90</v>
       </c>
       <c r="B81" t="s">
         <v>2</v>
@@ -2565,49 +2342,49 @@
         <v>4.2</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E81" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="B82" t="s">
         <v>2</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>208</v>
+        <v>126</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E82" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B83" t="s">
         <v>2</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>208</v>
+        <v>126</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E83" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
         <v>2</v>
@@ -2616,15 +2393,15 @@
         <v>2.5</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E84" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>176</v>
+        <v>94</v>
       </c>
       <c r="B85" t="s">
         <v>2</v>
@@ -2633,15 +2410,15 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E85" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
       <c r="B86" t="s">
         <v>2</v>
@@ -2650,15 +2427,15 @@
         <v>2.5</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E86" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>178</v>
+        <v>96</v>
       </c>
       <c r="B87" t="s">
         <v>2</v>
@@ -2667,15 +2444,15 @@
         <v>2.5</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E87" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>179</v>
+        <v>97</v>
       </c>
       <c r="B88" t="s">
         <v>2</v>
@@ -2684,15 +2461,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E88" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="B89" t="s">
         <v>2</v>
@@ -2701,15 +2478,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E89" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>181</v>
+        <v>99</v>
       </c>
       <c r="B90" t="s">
         <v>2</v>
@@ -2718,15 +2495,15 @@
         <v>4.2</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E90" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>182</v>
+        <v>100</v>
       </c>
       <c r="B91" t="s">
         <v>2</v>
@@ -2735,15 +2512,15 @@
         <v>4.2</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E91" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>183</v>
+        <v>101</v>
       </c>
       <c r="B92" t="s">
         <v>2</v>
@@ -2752,15 +2529,15 @@
         <v>4.3</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E92" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>184</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
         <v>2</v>
@@ -2769,15 +2546,15 @@
         <v>4.3</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E93" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>103</v>
       </c>
       <c r="B94" t="s">
         <v>2</v>
@@ -2786,15 +2563,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E94" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>186</v>
+        <v>104</v>
       </c>
       <c r="B95" t="s">
         <v>2</v>
@@ -2803,15 +2580,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E95" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>187</v>
+        <v>105</v>
       </c>
       <c r="B96" t="s">
         <v>2</v>
@@ -2820,15 +2597,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E96" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>188</v>
+        <v>106</v>
       </c>
       <c r="B97" t="s">
         <v>2</v>
@@ -2837,15 +2614,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E97" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="B98" t="s">
         <v>2</v>
@@ -2854,15 +2631,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E98" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>190</v>
+        <v>108</v>
       </c>
       <c r="B99" t="s">
         <v>2</v>
@@ -2871,15 +2648,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E99" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>191</v>
+        <v>109</v>
       </c>
       <c r="B100" t="s">
         <v>2</v>
@@ -2888,15 +2665,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E100" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>110</v>
       </c>
       <c r="B101" t="s">
         <v>2</v>
@@ -2905,15 +2682,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E101" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>193</v>
+        <v>111</v>
       </c>
       <c r="B102" t="s">
         <v>2</v>
@@ -2922,15 +2699,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E102" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>194</v>
+        <v>112</v>
       </c>
       <c r="B103" t="s">
         <v>2</v>
@@ -2939,15 +2716,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E103" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>195</v>
+        <v>113</v>
       </c>
       <c r="B104" t="s">
         <v>2</v>
@@ -2956,15 +2733,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E104" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>196</v>
+        <v>114</v>
       </c>
       <c r="B105" t="s">
         <v>2</v>
@@ -2973,15 +2750,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E105" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>197</v>
+        <v>115</v>
       </c>
       <c r="B106" t="s">
         <v>2</v>
@@ -2990,15 +2767,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E106" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>198</v>
+        <v>116</v>
       </c>
       <c r="B107" t="s">
         <v>2</v>
@@ -3007,15 +2784,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E107" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>199</v>
+        <v>117</v>
       </c>
       <c r="B108" t="s">
         <v>2</v>
@@ -3024,15 +2801,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E108" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>200</v>
+        <v>118</v>
       </c>
       <c r="B109" t="s">
         <v>2</v>
@@ -3041,15 +2818,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E109" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>201</v>
+        <v>119</v>
       </c>
       <c r="B110" t="s">
         <v>2</v>
@@ -3058,15 +2835,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E110" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>202</v>
+        <v>120</v>
       </c>
       <c r="B111" t="s">
         <v>2</v>
@@ -3075,15 +2852,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E111" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>203</v>
+        <v>121</v>
       </c>
       <c r="B112" t="s">
         <v>2</v>
@@ -3092,27 +2869,27 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="E112" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A113" s="6"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>212</v>
+        <v>130</v>
       </c>
       <c r="B115" t="s">
         <v>3</v>
@@ -3121,15 +2898,15 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E115" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="B116" t="s">
         <v>3</v>
@@ -3138,15 +2915,15 @@
         <v>1.4</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E116" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>214</v>
+        <v>132</v>
       </c>
       <c r="B117" t="s">
         <v>3</v>
@@ -3155,15 +2932,15 @@
         <v>2.5</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E117" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>215</v>
+        <v>133</v>
       </c>
       <c r="B118" t="s">
         <v>3</v>
@@ -3172,15 +2949,15 @@
         <v>2.5</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E118" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>216</v>
+        <v>134</v>
       </c>
       <c r="B119" t="s">
         <v>3</v>
@@ -3189,15 +2966,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E119" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>217</v>
+        <v>135</v>
       </c>
       <c r="B120" t="s">
         <v>3</v>
@@ -3206,15 +2983,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E120" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>218</v>
+        <v>136</v>
       </c>
       <c r="B121" t="s">
         <v>3</v>
@@ -3223,15 +3000,15 @@
         <v>1.4</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E121" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>219</v>
+        <v>137</v>
       </c>
       <c r="B122" t="s">
         <v>3</v>
@@ -3240,15 +3017,15 @@
         <v>1.2</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E122" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>220</v>
+        <v>138</v>
       </c>
       <c r="B123" t="s">
         <v>3</v>
@@ -3257,15 +3034,15 @@
         <v>1.2</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E123" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>221</v>
+        <v>139</v>
       </c>
       <c r="B124" t="s">
         <v>3</v>
@@ -3274,15 +3051,15 @@
         <v>1.2</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E124" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>222</v>
+        <v>140</v>
       </c>
       <c r="B125" t="s">
         <v>3</v>
@@ -3291,15 +3068,15 @@
         <v>1.2</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E125" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>223</v>
+        <v>141</v>
       </c>
       <c r="B126" t="s">
         <v>3</v>
@@ -3308,15 +3085,15 @@
         <v>1.2</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E126" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>224</v>
+        <v>142</v>
       </c>
       <c r="B127" t="s">
         <v>3</v>
@@ -3325,15 +3102,15 @@
         <v>1.2</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E127" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>225</v>
+        <v>143</v>
       </c>
       <c r="B128" t="s">
         <v>3</v>
@@ -3342,15 +3119,15 @@
         <v>2.4</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E128" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>226</v>
+        <v>144</v>
       </c>
       <c r="B129" t="s">
         <v>3</v>
@@ -3359,15 +3136,15 @@
         <v>2.4</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E129" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>227</v>
+        <v>145</v>
       </c>
       <c r="B130" t="s">
         <v>3</v>
@@ -3376,15 +3153,15 @@
         <v>2.4</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E130" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>228</v>
+        <v>146</v>
       </c>
       <c r="B131" t="s">
         <v>3</v>
@@ -3393,15 +3170,15 @@
         <v>3.8</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E131" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>229</v>
+        <v>147</v>
       </c>
       <c r="B132" t="s">
         <v>3</v>
@@ -3410,15 +3187,15 @@
         <v>3.8</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E132" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>211</v>
+        <v>129</v>
       </c>
       <c r="B133" t="s">
         <v>3</v>
@@ -3427,15 +3204,15 @@
         <v>4.13</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E133" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>210</v>
+        <v>128</v>
       </c>
       <c r="B134" t="s">
         <v>3</v>
@@ -3444,1078 +3221,1120 @@
         <v>4.13</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="E134" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A135" s="6"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>230</v>
+        <v>148</v>
       </c>
       <c r="B137" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C137" s="3">
         <v>2.5</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E137" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>235</v>
+        <v>153</v>
       </c>
       <c r="B138" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C138" s="3">
         <v>2.5</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E138" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>232</v>
+        <v>150</v>
       </c>
       <c r="B139" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C139" s="3">
         <v>2.5</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E139" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>231</v>
+        <v>149</v>
       </c>
       <c r="B140" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C140" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E140" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>236</v>
+        <v>154</v>
       </c>
       <c r="B141" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C141" s="3">
         <v>3.2</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E141" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>237</v>
+        <v>155</v>
       </c>
       <c r="B142" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C142" s="3">
         <v>3.2</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E142" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>238</v>
+        <v>156</v>
       </c>
       <c r="B143" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C143" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E143" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>233</v>
+        <v>151</v>
       </c>
       <c r="B144" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C144" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E144" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>234</v>
+        <v>152</v>
       </c>
       <c r="B145" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>241</v>
+        <v>159</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E145" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>239</v>
+        <v>157</v>
       </c>
       <c r="B146" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>241</v>
+        <v>159</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E146" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A147" s="6"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>242</v>
+        <v>160</v>
       </c>
       <c r="B149" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C149" s="3">
         <v>4.5</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E149" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>243</v>
+        <v>161</v>
       </c>
       <c r="B150" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C150" s="3">
         <v>4.5</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E150" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>244</v>
+        <v>162</v>
       </c>
       <c r="B151" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C151" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E151" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>245</v>
+        <v>163</v>
       </c>
       <c r="B152" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C152" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E152" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>263</v>
+        <v>181</v>
       </c>
       <c r="B153" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C153" s="3">
         <v>4.3</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E153" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>264</v>
+        <v>182</v>
       </c>
       <c r="B154" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C154" s="3">
         <v>4.3</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E154" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>265</v>
+        <v>183</v>
       </c>
       <c r="B155" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C155" s="3">
         <v>4.3</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E155" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>266</v>
+        <v>184</v>
       </c>
       <c r="B156" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C156" s="3">
         <v>4.2</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E156" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>267</v>
+        <v>185</v>
       </c>
       <c r="B157" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C157" s="3">
         <v>4.2</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E157" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>268</v>
+        <v>186</v>
       </c>
       <c r="B158" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C158" s="3">
         <v>4.2</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E158" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>289</v>
+        <v>207</v>
       </c>
       <c r="B159" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C159" s="3">
         <v>4.5</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E159" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>288</v>
+        <v>206</v>
       </c>
       <c r="B160" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C160" s="3">
         <v>4.5</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E160" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>287</v>
-      </c>
       <c r="B161" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C161" s="3">
         <v>4.5</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E161" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>286</v>
+        <v>204</v>
       </c>
       <c r="B162" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C162" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E162" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>285</v>
+        <v>203</v>
       </c>
       <c r="B163" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C163" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E163" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>284</v>
+        <v>202</v>
       </c>
       <c r="B164" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C164" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E164" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>283</v>
+        <v>201</v>
       </c>
       <c r="B165" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C165" s="3">
         <v>2.5</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E165" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>282</v>
+        <v>200</v>
       </c>
       <c r="B166" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C166" s="3">
         <v>2.5</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E166" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>281</v>
+        <v>199</v>
       </c>
       <c r="B167" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E167" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>280</v>
+        <v>198</v>
       </c>
       <c r="B168" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E168" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>279</v>
+        <v>197</v>
       </c>
       <c r="B169" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C169" s="3">
         <v>2.4</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E169" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>278</v>
+        <v>196</v>
       </c>
       <c r="B170" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C170" s="3">
         <v>2.4</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E170" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="B171" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C171" s="3">
         <v>4.1100000000000003</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E171" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="B172" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C172" s="3">
         <v>4.1100000000000003</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E172" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="B173" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C173" s="3">
         <v>4.1100000000000003</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E173" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="B174" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C174" s="3">
         <v>4.1100000000000003</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E174" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>273</v>
+        <v>191</v>
       </c>
       <c r="B175" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C175" s="3">
         <v>4.13</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E175" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>272</v>
+        <v>190</v>
       </c>
       <c r="B176" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C176" s="3">
         <v>4.13</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E176" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>271</v>
+        <v>189</v>
       </c>
       <c r="B177" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C177" s="3">
         <v>2.1</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E177" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>270</v>
+        <v>188</v>
       </c>
       <c r="B178" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C178" s="3">
         <v>4.7</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E178" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>262</v>
+        <v>180</v>
       </c>
       <c r="B179" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C179" s="3">
         <v>4.7</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E179" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>261</v>
+        <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C180" s="3">
         <v>4.7</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E180" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>260</v>
+        <v>178</v>
       </c>
       <c r="B181" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C181" s="3">
         <v>2.5</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E181" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>259</v>
+        <v>177</v>
       </c>
       <c r="B182" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C182" s="3">
         <v>2.5</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E182" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>258</v>
+        <v>176</v>
       </c>
       <c r="B183" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C183" s="3">
         <v>4.8</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E183" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>257</v>
+        <v>175</v>
       </c>
       <c r="B184" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C184" s="3">
         <v>4.8</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E184" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>256</v>
+        <v>174</v>
       </c>
       <c r="B185" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C185" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E185" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>255</v>
+        <v>173</v>
       </c>
       <c r="B186" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C186" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E186" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>254</v>
+        <v>172</v>
       </c>
       <c r="B187" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C187" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E187" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>253</v>
+        <v>171</v>
       </c>
       <c r="B188" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C188" s="3">
         <v>4.3</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E188" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>252</v>
+        <v>170</v>
       </c>
       <c r="B189" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C189" s="3">
         <v>4.3</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E189" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>251</v>
+        <v>169</v>
       </c>
       <c r="B190" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C190" s="3">
         <v>4.3</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E190" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>250</v>
+        <v>168</v>
       </c>
       <c r="B191" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C191" s="3">
         <v>4.2</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E191" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>249</v>
+        <v>167</v>
       </c>
       <c r="B192" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C192" s="3">
         <v>4.2</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E192" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>248</v>
+        <v>166</v>
       </c>
       <c r="B193" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C193" s="3">
         <v>4.2</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E193" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>247</v>
+        <v>165</v>
       </c>
       <c r="B194" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C194" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E194" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>246</v>
+        <v>164</v>
       </c>
       <c r="B195" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C195" s="3"/>
       <c r="D195" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E195" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="B196" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E196" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="B197" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C197" s="3"/>
       <c r="D197" s="3" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="E197" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C202" s="3"/>
-      <c r="D202" s="3"/>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C203" s="3"/>
-      <c r="D203" s="3"/>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C204" s="3"/>
-      <c r="D204" s="3"/>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>209</v>
+      </c>
+      <c r="B202" t="s">
+        <v>208</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>210</v>
+      </c>
+      <c r="B203" t="s">
+        <v>208</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>211</v>
+      </c>
+      <c r="B204" t="s">
+        <v>208</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C206" s="3"/>
       <c r="D206" s="3"/>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C207" s="3"/>
       <c r="D207" s="3"/>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C208" s="3"/>
       <c r="D208" s="3"/>
     </row>
-    <row r="209" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C209" s="3"/>
       <c r="D209" s="3"/>
     </row>
-    <row r="210" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C210" s="3"/>
       <c r="D210" s="3"/>
     </row>

</xml_diff>

<commit_message>
Updated the tests excel file
</commit_message>
<xml_diff>
--- a/Documents/test_requirement_map.xlsx
+++ b/Documents/test_requirement_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayan\Desktop\version 3\MarketSystemRepo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiha\OneDrive - post.bgu.ac.il\שולחן העבודה\My_Projects\Market_System\MarketSystemRepo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6071CFAD-12C5-4056-A204-E0F66490C1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B714D40F-5AFB-4641-A0F4-630619B712DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5AAA1A21-C7B5-4175-94AF-BD01E7E4DD12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5AAA1A21-C7B5-4175-94AF-BD01E7E4DD12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="228">
   <si>
     <t>Test</t>
   </si>
@@ -684,6 +684,42 @@
   </si>
   <si>
     <t xml:space="preserve">serviceLayer, PaymentProxy , DeliveryProxy </t>
+  </si>
+  <si>
+    <t>PurchasePolicyUnitTest</t>
+  </si>
+  <si>
+    <t>ValidateUserAllowedToCalculateStoreStrategyTestSuccess</t>
+  </si>
+  <si>
+    <t>ValidateUserAllowedToPurchaseStoreStrategyTestSuccess</t>
+  </si>
+  <si>
+    <t>ValidateUserAllowedToPurchaseStoreStrategyTestFail</t>
+  </si>
+  <si>
+    <t>ValidateUserAllowedToPurchaseProductStrategyTestSuccess</t>
+  </si>
+  <si>
+    <t>AlcoholAgeStoreStrategySuccess</t>
+  </si>
+  <si>
+    <t>QuantityLessThanStoreStrategySuccess</t>
+  </si>
+  <si>
+    <t>MaximumPolicyTestSuccess</t>
+  </si>
+  <si>
+    <t>4.2 II</t>
+  </si>
+  <si>
+    <t>2 b</t>
+  </si>
+  <si>
+    <t>1 c</t>
+  </si>
+  <si>
+    <t>StoreRepo, Purchase Policy, Purchase Strategy, Product, Store</t>
   </si>
 </sst>
 </file>
@@ -694,7 +730,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -702,7 +738,7 @@
       <u/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -711,14 +747,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -775,7 +811,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1071,22 +1107,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547AF65F-50E2-4545-8A86-E31EA8FDF2EA}">
-  <dimension ref="A1:E210"/>
+  <dimension ref="A1:E213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E204" sqref="E204"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="75.296875" customWidth="1"/>
-    <col min="2" max="2" width="35.296875" customWidth="1"/>
-    <col min="3" max="3" width="32.19921875" customWidth="1"/>
+    <col min="1" max="1" width="75.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="48.09765625" customWidth="1"/>
+    <col min="5" max="5" width="48.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1103,21 +1139,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1134,7 +1170,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1151,7 +1187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1168,7 +1204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1185,7 +1221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1202,7 +1238,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1219,7 +1255,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1236,7 +1272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1253,7 +1289,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1270,7 +1306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1287,7 +1323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1304,7 +1340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1321,7 +1357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1338,7 +1374,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1355,7 +1391,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1372,7 +1408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1389,7 +1425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1406,7 +1442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1423,7 +1459,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1440,7 +1476,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1457,7 +1493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1474,7 +1510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1491,7 +1527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1508,7 +1544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1525,7 +1561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1542,7 +1578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1559,19 +1595,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A30" s="6"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1588,7 +1624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A33" s="6"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
@@ -1598,7 +1634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>42</v>
       </c>
@@ -1615,7 +1651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1632,7 +1668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1649,7 +1685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1666,7 +1702,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1683,7 +1719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1700,7 +1736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -1717,7 +1753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -1734,7 +1770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -1751,19 +1787,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A43" s="6"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1780,7 +1816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1797,7 +1833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1814,7 +1850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1831,7 +1867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1848,7 +1884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -1865,19 +1901,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A51" s="6"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1894,7 +1930,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -1911,7 +1947,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1928,7 +1964,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1945,7 +1981,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1962,7 +1998,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1979,7 +2015,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -1996,7 +2032,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -2013,7 +2049,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -2030,7 +2066,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -2047,19 +2083,19 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A63" s="6"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -2076,7 +2112,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -2093,7 +2129,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -2110,7 +2146,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -2127,7 +2163,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -2144,7 +2180,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -2161,7 +2197,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -2178,7 +2214,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -2195,7 +2231,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -2212,7 +2248,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -2229,7 +2265,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -2246,7 +2282,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -2263,7 +2299,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -2280,7 +2316,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -2297,7 +2333,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -2314,7 +2350,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>89</v>
       </c>
@@ -2331,7 +2367,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>90</v>
       </c>
@@ -2348,7 +2384,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -2365,7 +2401,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>92</v>
       </c>
@@ -2382,7 +2418,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>93</v>
       </c>
@@ -2399,7 +2435,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -2416,7 +2452,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>95</v>
       </c>
@@ -2433,7 +2469,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>96</v>
       </c>
@@ -2450,7 +2486,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>97</v>
       </c>
@@ -2467,7 +2503,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>98</v>
       </c>
@@ -2484,7 +2520,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>99</v>
       </c>
@@ -2501,7 +2537,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>100</v>
       </c>
@@ -2518,7 +2554,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -2535,7 +2571,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -2552,7 +2588,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>103</v>
       </c>
@@ -2569,7 +2605,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>104</v>
       </c>
@@ -2586,7 +2622,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>105</v>
       </c>
@@ -2603,7 +2639,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>106</v>
       </c>
@@ -2620,7 +2656,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -2637,7 +2673,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>108</v>
       </c>
@@ -2654,7 +2690,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>109</v>
       </c>
@@ -2671,7 +2707,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>110</v>
       </c>
@@ -2688,7 +2724,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>111</v>
       </c>
@@ -2705,7 +2741,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>112</v>
       </c>
@@ -2722,7 +2758,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -2739,7 +2775,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>114</v>
       </c>
@@ -2756,7 +2792,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>115</v>
       </c>
@@ -2773,7 +2809,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>116</v>
       </c>
@@ -2790,7 +2826,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -2807,7 +2843,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>118</v>
       </c>
@@ -2824,7 +2860,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -2841,7 +2877,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>120</v>
       </c>
@@ -2858,7 +2894,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -2875,19 +2911,19 @@
         <v>123</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A113" s="6"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -2904,7 +2940,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>131</v>
       </c>
@@ -2921,7 +2957,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>132</v>
       </c>
@@ -2938,7 +2974,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>133</v>
       </c>
@@ -2955,7 +2991,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>134</v>
       </c>
@@ -2972,7 +3008,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>135</v>
       </c>
@@ -2989,7 +3025,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -3006,7 +3042,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>137</v>
       </c>
@@ -3023,7 +3059,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>138</v>
       </c>
@@ -3040,7 +3076,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>139</v>
       </c>
@@ -3057,7 +3093,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>140</v>
       </c>
@@ -3074,7 +3110,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -3091,7 +3127,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>142</v>
       </c>
@@ -3108,7 +3144,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>143</v>
       </c>
@@ -3125,7 +3161,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -3142,7 +3178,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>145</v>
       </c>
@@ -3159,7 +3195,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>146</v>
       </c>
@@ -3176,7 +3212,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>147</v>
       </c>
@@ -3193,7 +3229,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -3210,7 +3246,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>128</v>
       </c>
@@ -3227,19 +3263,19 @@
         <v>127</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A135" s="6"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>148</v>
       </c>
@@ -3256,7 +3292,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>153</v>
       </c>
@@ -3273,7 +3309,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>150</v>
       </c>
@@ -3290,7 +3326,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>149</v>
       </c>
@@ -3307,7 +3343,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>154</v>
       </c>
@@ -3324,7 +3360,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>155</v>
       </c>
@@ -3341,7 +3377,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>156</v>
       </c>
@@ -3358,7 +3394,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -3375,7 +3411,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>152</v>
       </c>
@@ -3392,7 +3428,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>157</v>
       </c>
@@ -3409,19 +3445,19 @@
         <v>123</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A147" s="6"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>160</v>
       </c>
@@ -3438,7 +3474,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>161</v>
       </c>
@@ -3455,7 +3491,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>162</v>
       </c>
@@ -3472,7 +3508,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>163</v>
       </c>
@@ -3489,7 +3525,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>181</v>
       </c>
@@ -3506,7 +3542,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>182</v>
       </c>
@@ -3523,7 +3559,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>183</v>
       </c>
@@ -3540,7 +3576,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>184</v>
       </c>
@@ -3557,7 +3593,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>185</v>
       </c>
@@ -3574,7 +3610,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>186</v>
       </c>
@@ -3591,7 +3627,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>207</v>
       </c>
@@ -3608,7 +3644,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>206</v>
       </c>
@@ -3625,7 +3661,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>205</v>
       </c>
@@ -3642,7 +3678,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>204</v>
       </c>
@@ -3659,7 +3695,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>203</v>
       </c>
@@ -3676,7 +3712,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>202</v>
       </c>
@@ -3693,7 +3729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>201</v>
       </c>
@@ -3710,7 +3746,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>200</v>
       </c>
@@ -3727,14 +3763,16 @@
         <v>123</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>199</v>
       </c>
       <c r="B167" t="s">
         <v>4</v>
       </c>
-      <c r="C167" s="3"/>
+      <c r="C167" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="D167" s="3" t="s">
         <v>158</v>
       </c>
@@ -3742,14 +3780,16 @@
         <v>123</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>198</v>
       </c>
       <c r="B168" t="s">
         <v>4</v>
       </c>
-      <c r="C168" s="3"/>
+      <c r="C168" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="D168" s="3" t="s">
         <v>158</v>
       </c>
@@ -3757,7 +3797,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>197</v>
       </c>
@@ -3774,7 +3814,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>196</v>
       </c>
@@ -3791,7 +3831,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>195</v>
       </c>
@@ -3808,7 +3848,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>194</v>
       </c>
@@ -3825,7 +3865,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>193</v>
       </c>
@@ -3842,7 +3882,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>192</v>
       </c>
@@ -3859,7 +3899,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>191</v>
       </c>
@@ -3876,7 +3916,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>190</v>
       </c>
@@ -3893,7 +3933,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>189</v>
       </c>
@@ -3910,7 +3950,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>188</v>
       </c>
@@ -3927,7 +3967,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -3944,7 +3984,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -3961,7 +4001,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>178</v>
       </c>
@@ -3978,7 +4018,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>177</v>
       </c>
@@ -3995,7 +4035,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>176</v>
       </c>
@@ -4012,7 +4052,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>175</v>
       </c>
@@ -4029,7 +4069,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>174</v>
       </c>
@@ -4046,7 +4086,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>173</v>
       </c>
@@ -4063,7 +4103,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>172</v>
       </c>
@@ -4080,7 +4120,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>171</v>
       </c>
@@ -4097,7 +4137,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>170</v>
       </c>
@@ -4114,7 +4154,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>169</v>
       </c>
@@ -4131,7 +4171,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>168</v>
       </c>
@@ -4148,7 +4188,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>167</v>
       </c>
@@ -4165,7 +4205,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>166</v>
       </c>
@@ -4182,7 +4222,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>165</v>
       </c>
@@ -4199,7 +4239,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>164</v>
       </c>
@@ -4214,7 +4254,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>187</v>
       </c>
@@ -4229,7 +4269,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>187</v>
       </c>
@@ -4244,26 +4284,26 @@
         <v>123</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>209</v>
       </c>
@@ -4280,7 +4320,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>210</v>
       </c>
@@ -4297,7 +4337,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>211</v>
       </c>
@@ -4314,29 +4354,135 @@
         <v>215</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="C206" s="3"/>
       <c r="D206" s="3"/>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C207" s="3"/>
-      <c r="D207" s="3"/>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C208" s="3"/>
-      <c r="D208" s="3"/>
-    </row>
-    <row r="209" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C209" s="3"/>
-      <c r="D209" s="3"/>
-    </row>
-    <row r="210" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C210" s="3"/>
-      <c r="D210" s="3"/>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>217</v>
+      </c>
+      <c r="B207" t="s">
+        <v>216</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>218</v>
+      </c>
+      <c r="B208" t="s">
+        <v>216</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>219</v>
+      </c>
+      <c r="B209" t="s">
+        <v>216</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>220</v>
+      </c>
+      <c r="B210" t="s">
+        <v>216</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>221</v>
+      </c>
+      <c r="B211" t="s">
+        <v>216</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>222</v>
+      </c>
+      <c r="B212" t="s">
+        <v>216</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>223</v>
+      </c>
+      <c r="B213" t="s">
+        <v>216</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>227</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>